<commit_message>
just needs sign out
</commit_message>
<xml_diff>
--- a/CG_SK_Lab1/CG_SK_Lab1/testdb.xlsx
+++ b/CG_SK_Lab1/CG_SK_Lab1/testdb.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="18195" windowHeight="7740" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="18195" windowHeight="7740" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -160,6 +160,15 @@
   </si>
   <si>
     <t>Friday</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>Number of Multiples</t>
+  </si>
+  <si>
+    <t>excusal</t>
   </si>
 </sst>
 </file>
@@ -201,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -209,6 +218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -915,10 +925,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -926,24 +936,58 @@
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="2">
         <v>38751.524259259262</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4">
+        <v>38751</v>
+      </c>
+      <c r="E2" s="5">
+        <f>MATCH("*",A2:A3,-1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2">
+        <v>41333</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="4">
+        <v>41333</v>
+      </c>
     </row>
   </sheetData>
   <customSheetViews>
@@ -960,7 +1004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
works...thats all that matters
</commit_message>
<xml_diff>
--- a/CG_SK_Lab1/CG_SK_Lab1/testdb.xlsx
+++ b/CG_SK_Lab1/CG_SK_Lab1/testdb.xlsx
@@ -16,13 +16,13 @@
   </sheets>
   <calcPr calcId="125725"/>
   <customWorkbookViews>
-    <customWorkbookView name="Network Student - Personal View" guid="{292070CA-CCC0-4443-AE30-5245732CEFEF}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1244" windowHeight="535" activeSheetId="2"/>
+    <customWorkbookView name="Network Student - Personal View" guid="{292070CA-CCC0-4443-AE30-5245732CEFEF}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="871" windowHeight="678" activeSheetId="6"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -161,6 +161,15 @@
   <si>
     <t>Friday</t>
   </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>Number of Multiples</t>
+  </si>
+  <si>
+    <t>excusal</t>
+  </si>
 </sst>
 </file>
 
@@ -201,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -209,6 +218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -216,6 +226,4375 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" guid="{6A088286-0EEB-47B9-8096-03EF60C01445}" diskRevisions="1" revisionId="402" version="5">
+  <header guid="{CDC0E8B4-BCE5-4D3F-8424-F8C784956298}" dateTime="2013-02-28T23:21:13" maxSheetId="7" userName="Network Student" r:id="rId1">
+    <sheetIdMap count="6">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{35DA0982-C5CD-4FE9-BCD2-1277FED1C2A0}" dateTime="2013-02-28T23:24:06" maxSheetId="7" userName="Network Student" r:id="rId2" minRId="1">
+    <sheetIdMap count="6">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{07C59B97-6326-40DD-9EDD-B2F9200380FB}" dateTime="2013-02-28T23:24:24" maxSheetId="7" userName="Network Student" r:id="rId3" minRId="2" maxRId="191">
+    <sheetIdMap count="6">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{75126F2E-4F5C-48EE-88DD-C6E32F8F7E3A}" dateTime="2013-02-28T23:26:07" maxSheetId="7" userName="Network Student" r:id="rId4" minRId="192" maxRId="380">
+    <sheetIdMap count="6">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{6A088286-0EEB-47B9-8096-03EF60C01445}" dateTime="2013-02-28T23:31:17" maxSheetId="7" userName="Network Student" r:id="rId5" minRId="381" maxRId="402">
+    <sheetIdMap count="6">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+    </sheetIdMap>
+  </header>
+</headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rrc rId="381" sId="6" ref="A97:XFD97" action="deleteRow">
+    <rfmt sheetId="6" xfDxf="1" sqref="A97:XFD97" start="0" length="0"/>
+    <rcc rId="0" sId="6">
+      <nc r="A97" t="inlineStr">
+        <is>
+          <t>dinner</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="6" dxf="1" numFmtId="19">
+      <nc r="B97">
+        <v>41333</v>
+      </nc>
+      <ndxf>
+        <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="6">
+      <nc r="C97" t="inlineStr">
+        <is>
+          <t>To be determined</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="6">
+      <nc r="D97">
+        <v>41333</v>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="6">
+      <nc r="E97" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </nc>
+    </rcc>
+  </rrc>
+  <rrc rId="382" sId="6" ref="A96:XFD96" action="deleteRow">
+    <rfmt sheetId="6" xfDxf="1" sqref="A96:XFD96" start="0" length="0"/>
+    <rcc rId="0" sId="6">
+      <nc r="A96" t="inlineStr">
+        <is>
+          <t>lunch</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="6" dxf="1" numFmtId="19">
+      <nc r="B96">
+        <v>41333</v>
+      </nc>
+      <ndxf>
+        <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="6">
+      <nc r="C96">
+        <v>16</v>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="6">
+      <nc r="D96">
+        <v>41333</v>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="6">
+      <nc r="E96" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </nc>
+    </rcc>
+  </rrc>
+  <rrc rId="383" sId="6" ref="A95:XFD95" action="insertRow"/>
+  <rrc rId="384" sId="6" ref="A96:XFD96" action="deleteRow">
+    <rfmt sheetId="6" xfDxf="1" sqref="A96:XFD96" start="0" length="0"/>
+    <rcc rId="0" sId="6">
+      <nc r="A96" t="inlineStr">
+        <is>
+          <t>lunch</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="6" dxf="1" numFmtId="19">
+      <nc r="B96">
+        <v>41333</v>
+      </nc>
+      <ndxf>
+        <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      </ndxf>
+    </rcc>
+    <rcc rId="0" sId="6">
+      <nc r="C96">
+        <v>16</v>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="6">
+      <nc r="D96">
+        <v>41333</v>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="6">
+      <nc r="E96" t="inlineStr">
+        <is>
+          <t>Thursday</t>
+        </is>
+      </nc>
+    </rcc>
+  </rrc>
+  <rrc rId="385" sId="6" ref="A2:XFD2" action="insertRow"/>
+  <rrc rId="386" sId="6" ref="A2:XFD2" action="insertRow"/>
+  <rrc rId="387" sId="6" ref="A2:XFD2" action="insertRow"/>
+  <rcc rId="388" sId="6">
+    <nc r="A2" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="389" sId="6">
+    <nc r="A3" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="390" sId="6">
+    <nc r="A4" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="391" sId="6" odxf="1" dxf="1" numFmtId="19">
+    <nc r="B2">
+      <v>41302</v>
+    </nc>
+    <odxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </odxf>
+    <ndxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="392" sId="6" odxf="1" dxf="1" numFmtId="19">
+    <nc r="B3">
+      <v>41302</v>
+    </nc>
+    <odxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </odxf>
+    <ndxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="393" sId="6" odxf="1" dxf="1" numFmtId="19">
+    <nc r="B4">
+      <v>41302</v>
+    </nc>
+    <odxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </odxf>
+    <ndxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </ndxf>
+  </rcc>
+  <rcc rId="394" sId="6">
+    <nc r="C2">
+      <v>564</v>
+    </nc>
+  </rcc>
+  <rcc rId="395" sId="6">
+    <nc r="C3">
+      <v>564</v>
+    </nc>
+  </rcc>
+  <rcc rId="396" sId="6">
+    <nc r="C4">
+      <v>564</v>
+    </nc>
+  </rcc>
+  <rcc rId="397" sId="6">
+    <nc r="D2">
+      <v>41302</v>
+    </nc>
+  </rcc>
+  <rcc rId="398" sId="6">
+    <nc r="D3">
+      <v>41302</v>
+    </nc>
+  </rcc>
+  <rcc rId="399" sId="6">
+    <nc r="D4">
+      <v>41302</v>
+    </nc>
+  </rcc>
+  <rcc rId="400" sId="6">
+    <nc r="E2" t="inlineStr">
+      <is>
+        <t>Monday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="401" sId="6">
+    <nc r="E3" t="inlineStr">
+      <is>
+        <t>Monday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="402" sId="6">
+    <nc r="E4" t="inlineStr">
+      <is>
+        <t>Monday</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="2" sId="6">
+    <oc r="A2" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A2" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="3" sId="6">
+    <oc r="A3" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A3" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="4" sId="6" numFmtId="19">
+    <oc r="B3">
+      <v>41302</v>
+    </oc>
+    <nc r="B3">
+      <v>41303</v>
+    </nc>
+  </rcc>
+  <rcc rId="5" sId="6">
+    <oc r="D3">
+      <v>41302</v>
+    </oc>
+    <nc r="D3">
+      <v>41303</v>
+    </nc>
+  </rcc>
+  <rcc rId="6" sId="6">
+    <oc r="E3" t="inlineStr">
+      <is>
+        <t>Monday</t>
+      </is>
+    </oc>
+    <nc r="E3" t="inlineStr">
+      <is>
+        <t>Tuesday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="7" sId="6">
+    <oc r="A4" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A4" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="8" sId="6">
+    <oc r="A5" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A5" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="9" sId="6">
+    <oc r="A6" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A6" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="10" sId="6" numFmtId="19">
+    <oc r="B6">
+      <v>41303</v>
+    </oc>
+    <nc r="B6">
+      <v>41304</v>
+    </nc>
+  </rcc>
+  <rcc rId="11" sId="6">
+    <oc r="D6">
+      <v>41303</v>
+    </oc>
+    <nc r="D6">
+      <v>41304</v>
+    </nc>
+  </rcc>
+  <rcc rId="12" sId="6">
+    <oc r="E6" t="inlineStr">
+      <is>
+        <t>Tuesday</t>
+      </is>
+    </oc>
+    <nc r="E6" t="inlineStr">
+      <is>
+        <t>Wednesday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="13" sId="6">
+    <oc r="A7" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A7" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="14" sId="6">
+    <oc r="A8" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A8" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="15" sId="6">
+    <oc r="A9" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A9" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="16" sId="6" numFmtId="19">
+    <oc r="B9">
+      <v>41304</v>
+    </oc>
+    <nc r="B9">
+      <v>41305</v>
+    </nc>
+  </rcc>
+  <rcc rId="17" sId="6">
+    <oc r="D9">
+      <v>41304</v>
+    </oc>
+    <nc r="D9">
+      <v>41305</v>
+    </nc>
+  </rcc>
+  <rcc rId="18" sId="6">
+    <oc r="E9" t="inlineStr">
+      <is>
+        <t>Wednesday</t>
+      </is>
+    </oc>
+    <nc r="E9" t="inlineStr">
+      <is>
+        <t>Thursday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="19" sId="6">
+    <oc r="A10" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A10" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="20" sId="6">
+    <oc r="A11" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A11" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="21" sId="6">
+    <oc r="A12" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A12" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="22" sId="6" numFmtId="19">
+    <oc r="B12">
+      <v>41305</v>
+    </oc>
+    <nc r="B12">
+      <v>41306</v>
+    </nc>
+  </rcc>
+  <rcc rId="23" sId="6">
+    <oc r="D12">
+      <v>41305</v>
+    </oc>
+    <nc r="D12">
+      <v>41306</v>
+    </nc>
+  </rcc>
+  <rcc rId="24" sId="6">
+    <oc r="E12" t="inlineStr">
+      <is>
+        <t>Thursday</t>
+      </is>
+    </oc>
+    <nc r="E12" t="inlineStr">
+      <is>
+        <t>Friday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="25" sId="6">
+    <oc r="A13" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A13" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="26" sId="6">
+    <oc r="A14" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A14" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="27" sId="6">
+    <oc r="A15" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A15" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="28" sId="6" numFmtId="19">
+    <oc r="B15">
+      <v>41306</v>
+    </oc>
+    <nc r="B15">
+      <v>41307</v>
+    </nc>
+  </rcc>
+  <rcc rId="29" sId="6">
+    <oc r="D15">
+      <v>41306</v>
+    </oc>
+    <nc r="D15">
+      <v>41307</v>
+    </nc>
+  </rcc>
+  <rcc rId="30" sId="6">
+    <oc r="E15" t="inlineStr">
+      <is>
+        <t>Friday</t>
+      </is>
+    </oc>
+    <nc r="E15" t="inlineStr">
+      <is>
+        <t>Saturday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="31" sId="6">
+    <oc r="A16" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A16" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="32" sId="6">
+    <oc r="A17" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A17" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="33" sId="6">
+    <oc r="A18" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A18" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="34" sId="6" numFmtId="19">
+    <oc r="B18">
+      <v>41307</v>
+    </oc>
+    <nc r="B18">
+      <v>41308</v>
+    </nc>
+  </rcc>
+  <rcc rId="35" sId="6">
+    <oc r="D18">
+      <v>41307</v>
+    </oc>
+    <nc r="D18">
+      <v>41308</v>
+    </nc>
+  </rcc>
+  <rcc rId="36" sId="6">
+    <oc r="E18" t="inlineStr">
+      <is>
+        <t>Saturday</t>
+      </is>
+    </oc>
+    <nc r="E18" t="inlineStr">
+      <is>
+        <t>Sunday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="37" sId="6">
+    <oc r="A19" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A19" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="38" sId="6">
+    <oc r="A20" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A20" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="39" sId="6">
+    <oc r="A21" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A21" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="40" sId="6" numFmtId="19">
+    <oc r="B21">
+      <v>41308</v>
+    </oc>
+    <nc r="B21">
+      <v>41309</v>
+    </nc>
+  </rcc>
+  <rcc rId="41" sId="6">
+    <oc r="D21">
+      <v>41308</v>
+    </oc>
+    <nc r="D21">
+      <v>41309</v>
+    </nc>
+  </rcc>
+  <rcc rId="42" sId="6">
+    <oc r="E21" t="inlineStr">
+      <is>
+        <t>Sunday</t>
+      </is>
+    </oc>
+    <nc r="E21" t="inlineStr">
+      <is>
+        <t>Monday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="43" sId="6">
+    <oc r="A22" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A22" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="44" sId="6">
+    <oc r="A23" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A23" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="45" sId="6">
+    <oc r="A24" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A24" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="46" sId="6" numFmtId="19">
+    <oc r="B24">
+      <v>41309</v>
+    </oc>
+    <nc r="B24">
+      <v>41310</v>
+    </nc>
+  </rcc>
+  <rcc rId="47" sId="6">
+    <oc r="D24">
+      <v>41309</v>
+    </oc>
+    <nc r="D24">
+      <v>41310</v>
+    </nc>
+  </rcc>
+  <rcc rId="48" sId="6">
+    <oc r="E24" t="inlineStr">
+      <is>
+        <t>Monday</t>
+      </is>
+    </oc>
+    <nc r="E24" t="inlineStr">
+      <is>
+        <t>Tuesday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="49" sId="6">
+    <oc r="A25" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A25" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="50" sId="6">
+    <oc r="A26" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A26" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="51" sId="6">
+    <oc r="A27" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A27" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="52" sId="6" numFmtId="19">
+    <oc r="B27">
+      <v>41310</v>
+    </oc>
+    <nc r="B27">
+      <v>41311</v>
+    </nc>
+  </rcc>
+  <rcc rId="53" sId="6">
+    <oc r="D27">
+      <v>41310</v>
+    </oc>
+    <nc r="D27">
+      <v>41311</v>
+    </nc>
+  </rcc>
+  <rcc rId="54" sId="6">
+    <oc r="E27" t="inlineStr">
+      <is>
+        <t>Tuesday</t>
+      </is>
+    </oc>
+    <nc r="E27" t="inlineStr">
+      <is>
+        <t>Wednesday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="55" sId="6">
+    <oc r="A28" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A28" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="56" sId="6">
+    <oc r="A29" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A29" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="57" sId="6">
+    <oc r="A30" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A30" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="58" sId="6" numFmtId="19">
+    <oc r="B30">
+      <v>41311</v>
+    </oc>
+    <nc r="B30">
+      <v>41312</v>
+    </nc>
+  </rcc>
+  <rcc rId="59" sId="6">
+    <oc r="D30">
+      <v>41311</v>
+    </oc>
+    <nc r="D30">
+      <v>41312</v>
+    </nc>
+  </rcc>
+  <rcc rId="60" sId="6">
+    <oc r="E30" t="inlineStr">
+      <is>
+        <t>Wednesday</t>
+      </is>
+    </oc>
+    <nc r="E30" t="inlineStr">
+      <is>
+        <t>Thursday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="61" sId="6">
+    <oc r="A31" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A31" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="62" sId="6">
+    <oc r="A32" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A32" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="63" sId="6">
+    <oc r="A33" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A33" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="64" sId="6" numFmtId="19">
+    <oc r="B33">
+      <v>41312</v>
+    </oc>
+    <nc r="B33">
+      <v>41313</v>
+    </nc>
+  </rcc>
+  <rcc rId="65" sId="6">
+    <oc r="D33">
+      <v>41312</v>
+    </oc>
+    <nc r="D33">
+      <v>41313</v>
+    </nc>
+  </rcc>
+  <rcc rId="66" sId="6">
+    <oc r="E33" t="inlineStr">
+      <is>
+        <t>Thursday</t>
+      </is>
+    </oc>
+    <nc r="E33" t="inlineStr">
+      <is>
+        <t>Friday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="67" sId="6">
+    <oc r="A34" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A34" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="68" sId="6">
+    <oc r="A35" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A35" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="69" sId="6">
+    <oc r="A36" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A36" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="70" sId="6" numFmtId="19">
+    <oc r="B36">
+      <v>41313</v>
+    </oc>
+    <nc r="B36">
+      <v>41314</v>
+    </nc>
+  </rcc>
+  <rcc rId="71" sId="6">
+    <oc r="D36">
+      <v>41313</v>
+    </oc>
+    <nc r="D36">
+      <v>41314</v>
+    </nc>
+  </rcc>
+  <rcc rId="72" sId="6">
+    <oc r="E36" t="inlineStr">
+      <is>
+        <t>Friday</t>
+      </is>
+    </oc>
+    <nc r="E36" t="inlineStr">
+      <is>
+        <t>Saturday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="73" sId="6">
+    <oc r="A37" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A37" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="74" sId="6">
+    <oc r="A38" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A38" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="75" sId="6">
+    <oc r="A39" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A39" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="76" sId="6" numFmtId="19">
+    <oc r="B39">
+      <v>41314</v>
+    </oc>
+    <nc r="B39">
+      <v>41315</v>
+    </nc>
+  </rcc>
+  <rcc rId="77" sId="6">
+    <oc r="D39">
+      <v>41314</v>
+    </oc>
+    <nc r="D39">
+      <v>41315</v>
+    </nc>
+  </rcc>
+  <rcc rId="78" sId="6">
+    <oc r="E39" t="inlineStr">
+      <is>
+        <t>Saturday</t>
+      </is>
+    </oc>
+    <nc r="E39" t="inlineStr">
+      <is>
+        <t>Sunday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="79" sId="6">
+    <oc r="A40" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A40" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="80" sId="6">
+    <oc r="A41" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A41" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="81" sId="6">
+    <oc r="A42" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A42" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="82" sId="6" numFmtId="19">
+    <oc r="B42">
+      <v>41315</v>
+    </oc>
+    <nc r="B42">
+      <v>41316</v>
+    </nc>
+  </rcc>
+  <rcc rId="83" sId="6">
+    <oc r="D42">
+      <v>41315</v>
+    </oc>
+    <nc r="D42">
+      <v>41316</v>
+    </nc>
+  </rcc>
+  <rcc rId="84" sId="6">
+    <oc r="E42" t="inlineStr">
+      <is>
+        <t>Sunday</t>
+      </is>
+    </oc>
+    <nc r="E42" t="inlineStr">
+      <is>
+        <t>Monday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="85" sId="6">
+    <oc r="A43" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A43" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="86" sId="6">
+    <oc r="A44" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A44" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="87" sId="6">
+    <oc r="A45" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A45" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="88" sId="6" numFmtId="19">
+    <oc r="B45">
+      <v>41316</v>
+    </oc>
+    <nc r="B45">
+      <v>41317</v>
+    </nc>
+  </rcc>
+  <rcc rId="89" sId="6">
+    <oc r="D45">
+      <v>41316</v>
+    </oc>
+    <nc r="D45">
+      <v>41317</v>
+    </nc>
+  </rcc>
+  <rcc rId="90" sId="6">
+    <oc r="E45" t="inlineStr">
+      <is>
+        <t>Monday</t>
+      </is>
+    </oc>
+    <nc r="E45" t="inlineStr">
+      <is>
+        <t>Tuesday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="91" sId="6">
+    <oc r="A46" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A46" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="92" sId="6">
+    <oc r="A47" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A47" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="93" sId="6">
+    <oc r="A48" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A48" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="94" sId="6" numFmtId="19">
+    <oc r="B48">
+      <v>41317</v>
+    </oc>
+    <nc r="B48">
+      <v>41318</v>
+    </nc>
+  </rcc>
+  <rcc rId="95" sId="6">
+    <oc r="D48">
+      <v>41317</v>
+    </oc>
+    <nc r="D48">
+      <v>41318</v>
+    </nc>
+  </rcc>
+  <rcc rId="96" sId="6">
+    <oc r="E48" t="inlineStr">
+      <is>
+        <t>Tuesday</t>
+      </is>
+    </oc>
+    <nc r="E48" t="inlineStr">
+      <is>
+        <t>Wednesday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="97" sId="6">
+    <oc r="A49" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A49" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="98" sId="6">
+    <oc r="A50" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A50" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="99" sId="6">
+    <oc r="A51" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A51" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="100" sId="6" numFmtId="19">
+    <oc r="B51">
+      <v>41318</v>
+    </oc>
+    <nc r="B51">
+      <v>41319</v>
+    </nc>
+  </rcc>
+  <rcc rId="101" sId="6">
+    <oc r="D51">
+      <v>41318</v>
+    </oc>
+    <nc r="D51">
+      <v>41319</v>
+    </nc>
+  </rcc>
+  <rcc rId="102" sId="6">
+    <oc r="E51" t="inlineStr">
+      <is>
+        <t>Wednesday</t>
+      </is>
+    </oc>
+    <nc r="E51" t="inlineStr">
+      <is>
+        <t>Thursday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="103" sId="6">
+    <oc r="A52" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A52" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="104" sId="6">
+    <oc r="A53" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A53" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="105" sId="6">
+    <oc r="A54" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A54" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="106" sId="6" numFmtId="19">
+    <oc r="B54">
+      <v>41319</v>
+    </oc>
+    <nc r="B54">
+      <v>41320</v>
+    </nc>
+  </rcc>
+  <rcc rId="107" sId="6">
+    <oc r="D54">
+      <v>41319</v>
+    </oc>
+    <nc r="D54">
+      <v>41320</v>
+    </nc>
+  </rcc>
+  <rcc rId="108" sId="6">
+    <oc r="E54" t="inlineStr">
+      <is>
+        <t>Thursday</t>
+      </is>
+    </oc>
+    <nc r="E54" t="inlineStr">
+      <is>
+        <t>Friday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="109" sId="6">
+    <oc r="A55" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A55" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="110" sId="6">
+    <oc r="A56" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A56" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="111" sId="6">
+    <oc r="A57" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A57" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="112" sId="6" numFmtId="19">
+    <oc r="B57">
+      <v>41320</v>
+    </oc>
+    <nc r="B57">
+      <v>41321</v>
+    </nc>
+  </rcc>
+  <rcc rId="113" sId="6">
+    <oc r="D57">
+      <v>41320</v>
+    </oc>
+    <nc r="D57">
+      <v>41321</v>
+    </nc>
+  </rcc>
+  <rcc rId="114" sId="6">
+    <oc r="E57" t="inlineStr">
+      <is>
+        <t>Friday</t>
+      </is>
+    </oc>
+    <nc r="E57" t="inlineStr">
+      <is>
+        <t>Saturday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="115" sId="6">
+    <oc r="A58" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A58" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="116" sId="6">
+    <oc r="A59" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A59" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="117" sId="6">
+    <oc r="A60" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A60" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="118" sId="6" numFmtId="19">
+    <oc r="B60">
+      <v>41321</v>
+    </oc>
+    <nc r="B60">
+      <v>41322</v>
+    </nc>
+  </rcc>
+  <rcc rId="119" sId="6">
+    <oc r="D60">
+      <v>41321</v>
+    </oc>
+    <nc r="D60">
+      <v>41322</v>
+    </nc>
+  </rcc>
+  <rcc rId="120" sId="6">
+    <oc r="E60" t="inlineStr">
+      <is>
+        <t>Saturday</t>
+      </is>
+    </oc>
+    <nc r="E60" t="inlineStr">
+      <is>
+        <t>Sunday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="121" sId="6">
+    <oc r="A61" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A61" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="122" sId="6">
+    <oc r="A62" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A62" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="123" sId="6">
+    <oc r="A63" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A63" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="124" sId="6" numFmtId="19">
+    <oc r="B63">
+      <v>41322</v>
+    </oc>
+    <nc r="B63">
+      <v>41323</v>
+    </nc>
+  </rcc>
+  <rcc rId="125" sId="6">
+    <oc r="D63">
+      <v>41322</v>
+    </oc>
+    <nc r="D63">
+      <v>41323</v>
+    </nc>
+  </rcc>
+  <rcc rId="126" sId="6">
+    <oc r="E63" t="inlineStr">
+      <is>
+        <t>Sunday</t>
+      </is>
+    </oc>
+    <nc r="E63" t="inlineStr">
+      <is>
+        <t>Monday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="127" sId="6">
+    <oc r="A64" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A64" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="128" sId="6">
+    <oc r="A65" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A65" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="129" sId="6">
+    <oc r="A66" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A66" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="130" sId="6" numFmtId="19">
+    <oc r="B66">
+      <v>41323</v>
+    </oc>
+    <nc r="B66">
+      <v>41324</v>
+    </nc>
+  </rcc>
+  <rcc rId="131" sId="6">
+    <oc r="D66">
+      <v>41323</v>
+    </oc>
+    <nc r="D66">
+      <v>41324</v>
+    </nc>
+  </rcc>
+  <rcc rId="132" sId="6">
+    <oc r="E66" t="inlineStr">
+      <is>
+        <t>Monday</t>
+      </is>
+    </oc>
+    <nc r="E66" t="inlineStr">
+      <is>
+        <t>Tuesday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="133" sId="6">
+    <oc r="A67" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A67" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="134" sId="6">
+    <oc r="A68" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A68" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="135" sId="6">
+    <oc r="A69" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A69" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="136" sId="6" numFmtId="19">
+    <oc r="B69">
+      <v>41324</v>
+    </oc>
+    <nc r="B69">
+      <v>41325</v>
+    </nc>
+  </rcc>
+  <rcc rId="137" sId="6">
+    <oc r="D69">
+      <v>41324</v>
+    </oc>
+    <nc r="D69">
+      <v>41325</v>
+    </nc>
+  </rcc>
+  <rcc rId="138" sId="6">
+    <oc r="E69" t="inlineStr">
+      <is>
+        <t>Tuesday</t>
+      </is>
+    </oc>
+    <nc r="E69" t="inlineStr">
+      <is>
+        <t>Wednesday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="139" sId="6">
+    <oc r="A70" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A70" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="140" sId="6">
+    <oc r="A71" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A71" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="141" sId="6">
+    <oc r="A72" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A72" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="142" sId="6" numFmtId="19">
+    <oc r="B72">
+      <v>41325</v>
+    </oc>
+    <nc r="B72">
+      <v>41326</v>
+    </nc>
+  </rcc>
+  <rcc rId="143" sId="6">
+    <oc r="D72">
+      <v>41325</v>
+    </oc>
+    <nc r="D72">
+      <v>41326</v>
+    </nc>
+  </rcc>
+  <rcc rId="144" sId="6">
+    <oc r="E72" t="inlineStr">
+      <is>
+        <t>Wednesday</t>
+      </is>
+    </oc>
+    <nc r="E72" t="inlineStr">
+      <is>
+        <t>Thursday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="145" sId="6">
+    <oc r="A73" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A73" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="146" sId="6">
+    <oc r="A74" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A74" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="147" sId="6">
+    <oc r="A75" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A75" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="148" sId="6" numFmtId="19">
+    <oc r="B75">
+      <v>41326</v>
+    </oc>
+    <nc r="B75">
+      <v>41327</v>
+    </nc>
+  </rcc>
+  <rcc rId="149" sId="6">
+    <oc r="D75">
+      <v>41326</v>
+    </oc>
+    <nc r="D75">
+      <v>41327</v>
+    </nc>
+  </rcc>
+  <rcc rId="150" sId="6">
+    <oc r="E75" t="inlineStr">
+      <is>
+        <t>Thursday</t>
+      </is>
+    </oc>
+    <nc r="E75" t="inlineStr">
+      <is>
+        <t>Friday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="151" sId="6">
+    <oc r="A76" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A76" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="152" sId="6">
+    <oc r="A77" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A77" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="153" sId="6">
+    <oc r="A78" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A78" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="154" sId="6" numFmtId="19">
+    <oc r="B78">
+      <v>41327</v>
+    </oc>
+    <nc r="B78">
+      <v>41328</v>
+    </nc>
+  </rcc>
+  <rcc rId="155" sId="6">
+    <oc r="D78">
+      <v>41327</v>
+    </oc>
+    <nc r="D78">
+      <v>41328</v>
+    </nc>
+  </rcc>
+  <rcc rId="156" sId="6">
+    <oc r="E78" t="inlineStr">
+      <is>
+        <t>Friday</t>
+      </is>
+    </oc>
+    <nc r="E78" t="inlineStr">
+      <is>
+        <t>Saturday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="157" sId="6">
+    <oc r="A79" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A79" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="158" sId="6">
+    <oc r="A80" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A80" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="159" sId="6">
+    <oc r="A81" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A81" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="160" sId="6" numFmtId="19">
+    <oc r="B81">
+      <v>41328</v>
+    </oc>
+    <nc r="B81">
+      <v>41329</v>
+    </nc>
+  </rcc>
+  <rcc rId="161" sId="6">
+    <oc r="D81">
+      <v>41328</v>
+    </oc>
+    <nc r="D81">
+      <v>41329</v>
+    </nc>
+  </rcc>
+  <rcc rId="162" sId="6">
+    <oc r="E81" t="inlineStr">
+      <is>
+        <t>Saturday</t>
+      </is>
+    </oc>
+    <nc r="E81" t="inlineStr">
+      <is>
+        <t>Sunday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="163" sId="6">
+    <oc r="A82" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A82" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="164" sId="6">
+    <oc r="A83" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A83" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="165" sId="6">
+    <oc r="A84" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A84" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="166" sId="6" numFmtId="19">
+    <oc r="B84">
+      <v>41329</v>
+    </oc>
+    <nc r="B84">
+      <v>41330</v>
+    </nc>
+  </rcc>
+  <rcc rId="167" sId="6">
+    <oc r="D84">
+      <v>41329</v>
+    </oc>
+    <nc r="D84">
+      <v>41330</v>
+    </nc>
+  </rcc>
+  <rcc rId="168" sId="6">
+    <oc r="E84" t="inlineStr">
+      <is>
+        <t>Sunday</t>
+      </is>
+    </oc>
+    <nc r="E84" t="inlineStr">
+      <is>
+        <t>Monday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="169" sId="6">
+    <oc r="A85" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A85" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="170" sId="6">
+    <oc r="A86" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A86" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="171" sId="6">
+    <oc r="A87" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A87" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="172" sId="6" numFmtId="19">
+    <oc r="B87">
+      <v>41330</v>
+    </oc>
+    <nc r="B87">
+      <v>41331</v>
+    </nc>
+  </rcc>
+  <rcc rId="173" sId="6">
+    <oc r="D87">
+      <v>41330</v>
+    </oc>
+    <nc r="D87">
+      <v>41331</v>
+    </nc>
+  </rcc>
+  <rcc rId="174" sId="6">
+    <oc r="E87" t="inlineStr">
+      <is>
+        <t>Monday</t>
+      </is>
+    </oc>
+    <nc r="E87" t="inlineStr">
+      <is>
+        <t>Tuesday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="175" sId="6">
+    <oc r="A88" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A88" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="176" sId="6">
+    <oc r="A89" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A89" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="177" sId="6">
+    <oc r="A90" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A90" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="178" sId="6" numFmtId="19">
+    <oc r="B90">
+      <v>41331</v>
+    </oc>
+    <nc r="B90">
+      <v>41332</v>
+    </nc>
+  </rcc>
+  <rcc rId="179" sId="6">
+    <oc r="D90">
+      <v>41331</v>
+    </oc>
+    <nc r="D90">
+      <v>41332</v>
+    </nc>
+  </rcc>
+  <rcc rId="180" sId="6">
+    <oc r="E90" t="inlineStr">
+      <is>
+        <t>Tuesday</t>
+      </is>
+    </oc>
+    <nc r="E90" t="inlineStr">
+      <is>
+        <t>Wednesday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="181" sId="6">
+    <oc r="A91" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A91" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="182" sId="6">
+    <oc r="A92" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A92" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="183" sId="6">
+    <oc r="A93" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A93" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="184" sId="6" numFmtId="19">
+    <oc r="B93">
+      <v>41332</v>
+    </oc>
+    <nc r="B93">
+      <v>41333</v>
+    </nc>
+  </rcc>
+  <rcc rId="185" sId="6">
+    <oc r="D93">
+      <v>41332</v>
+    </oc>
+    <nc r="D93">
+      <v>41333</v>
+    </nc>
+  </rcc>
+  <rcc rId="186" sId="6">
+    <oc r="E93" t="inlineStr">
+      <is>
+        <t>Wednesday</t>
+      </is>
+    </oc>
+    <nc r="E93" t="inlineStr">
+      <is>
+        <t>Thursday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="187" sId="6">
+    <oc r="A94" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A94" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="188" sId="6">
+    <oc r="A95" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A95" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="189" sId="6">
+    <oc r="C95">
+      <v>564</v>
+    </oc>
+    <nc r="C95">
+      <v>16</v>
+    </nc>
+  </rcc>
+  <rcc rId="190" sId="6">
+    <oc r="A96" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A96" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="191" sId="6">
+    <oc r="C97">
+      <v>14</v>
+    </oc>
+    <nc r="C97" t="inlineStr">
+      <is>
+        <t>To be determined</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="6" sqref="D97" start="0" length="0">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="6" sqref="D97">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog111.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="1" sId="6">
+    <nc r="C97">
+      <v>14</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog1111.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</file>
+
+<file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rcc rId="192" sId="6">
+    <oc r="A2" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A2" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="193" sId="6" numFmtId="19">
+    <oc r="B2">
+      <v>41302</v>
+    </oc>
+    <nc r="B2">
+      <v>41303</v>
+    </nc>
+  </rcc>
+  <rcc rId="194" sId="6">
+    <oc r="D2">
+      <v>41302</v>
+    </oc>
+    <nc r="D2">
+      <v>41303</v>
+    </nc>
+  </rcc>
+  <rcc rId="195" sId="6">
+    <oc r="E2" t="inlineStr">
+      <is>
+        <t>Monday</t>
+      </is>
+    </oc>
+    <nc r="E2" t="inlineStr">
+      <is>
+        <t>Tuesday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="196" sId="6">
+    <oc r="A3" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A3" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="197" sId="6">
+    <oc r="A4" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A4" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="198" sId="6">
+    <oc r="A5" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A5" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="199" sId="6" numFmtId="19">
+    <oc r="B5">
+      <v>41303</v>
+    </oc>
+    <nc r="B5">
+      <v>41304</v>
+    </nc>
+  </rcc>
+  <rcc rId="200" sId="6">
+    <oc r="D5">
+      <v>41303</v>
+    </oc>
+    <nc r="D5">
+      <v>41304</v>
+    </nc>
+  </rcc>
+  <rcc rId="201" sId="6">
+    <oc r="E5" t="inlineStr">
+      <is>
+        <t>Tuesday</t>
+      </is>
+    </oc>
+    <nc r="E5" t="inlineStr">
+      <is>
+        <t>Wednesday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="202" sId="6">
+    <oc r="A6" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A6" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="203" sId="6">
+    <oc r="A7" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A7" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="204" sId="6">
+    <oc r="A8" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A8" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="205" sId="6" numFmtId="19">
+    <oc r="B8">
+      <v>41304</v>
+    </oc>
+    <nc r="B8">
+      <v>41305</v>
+    </nc>
+  </rcc>
+  <rcc rId="206" sId="6">
+    <oc r="D8">
+      <v>41304</v>
+    </oc>
+    <nc r="D8">
+      <v>41305</v>
+    </nc>
+  </rcc>
+  <rcc rId="207" sId="6">
+    <oc r="E8" t="inlineStr">
+      <is>
+        <t>Wednesday</t>
+      </is>
+    </oc>
+    <nc r="E8" t="inlineStr">
+      <is>
+        <t>Thursday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="208" sId="6">
+    <oc r="A9" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A9" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="209" sId="6">
+    <oc r="A10" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A10" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="210" sId="6">
+    <oc r="A11" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A11" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="211" sId="6" numFmtId="19">
+    <oc r="B11">
+      <v>41305</v>
+    </oc>
+    <nc r="B11">
+      <v>41306</v>
+    </nc>
+  </rcc>
+  <rcc rId="212" sId="6">
+    <oc r="D11">
+      <v>41305</v>
+    </oc>
+    <nc r="D11">
+      <v>41306</v>
+    </nc>
+  </rcc>
+  <rcc rId="213" sId="6">
+    <oc r="E11" t="inlineStr">
+      <is>
+        <t>Thursday</t>
+      </is>
+    </oc>
+    <nc r="E11" t="inlineStr">
+      <is>
+        <t>Friday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="214" sId="6">
+    <oc r="A12" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A12" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="215" sId="6">
+    <oc r="A13" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A13" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="216" sId="6">
+    <oc r="A14" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A14" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="217" sId="6" numFmtId="19">
+    <oc r="B14">
+      <v>41306</v>
+    </oc>
+    <nc r="B14">
+      <v>41307</v>
+    </nc>
+  </rcc>
+  <rcc rId="218" sId="6">
+    <oc r="D14">
+      <v>41306</v>
+    </oc>
+    <nc r="D14">
+      <v>41307</v>
+    </nc>
+  </rcc>
+  <rcc rId="219" sId="6">
+    <oc r="E14" t="inlineStr">
+      <is>
+        <t>Friday</t>
+      </is>
+    </oc>
+    <nc r="E14" t="inlineStr">
+      <is>
+        <t>Saturday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="220" sId="6">
+    <oc r="A15" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A15" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="221" sId="6">
+    <oc r="A16" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A16" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="222" sId="6">
+    <oc r="A17" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A17" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="223" sId="6" numFmtId="19">
+    <oc r="B17">
+      <v>41307</v>
+    </oc>
+    <nc r="B17">
+      <v>41308</v>
+    </nc>
+  </rcc>
+  <rcc rId="224" sId="6">
+    <oc r="D17">
+      <v>41307</v>
+    </oc>
+    <nc r="D17">
+      <v>41308</v>
+    </nc>
+  </rcc>
+  <rcc rId="225" sId="6">
+    <oc r="E17" t="inlineStr">
+      <is>
+        <t>Saturday</t>
+      </is>
+    </oc>
+    <nc r="E17" t="inlineStr">
+      <is>
+        <t>Sunday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="226" sId="6">
+    <oc r="A18" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A18" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="227" sId="6">
+    <oc r="A19" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A19" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="228" sId="6">
+    <oc r="A20" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A20" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="229" sId="6" numFmtId="19">
+    <oc r="B20">
+      <v>41308</v>
+    </oc>
+    <nc r="B20">
+      <v>41309</v>
+    </nc>
+  </rcc>
+  <rcc rId="230" sId="6">
+    <oc r="D20">
+      <v>41308</v>
+    </oc>
+    <nc r="D20">
+      <v>41309</v>
+    </nc>
+  </rcc>
+  <rcc rId="231" sId="6">
+    <oc r="E20" t="inlineStr">
+      <is>
+        <t>Sunday</t>
+      </is>
+    </oc>
+    <nc r="E20" t="inlineStr">
+      <is>
+        <t>Monday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="232" sId="6">
+    <oc r="A21" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A21" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="233" sId="6">
+    <oc r="A22" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A22" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="234" sId="6">
+    <oc r="A23" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A23" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="235" sId="6" numFmtId="19">
+    <oc r="B23">
+      <v>41309</v>
+    </oc>
+    <nc r="B23">
+      <v>41310</v>
+    </nc>
+  </rcc>
+  <rcc rId="236" sId="6">
+    <oc r="D23">
+      <v>41309</v>
+    </oc>
+    <nc r="D23">
+      <v>41310</v>
+    </nc>
+  </rcc>
+  <rcc rId="237" sId="6">
+    <oc r="E23" t="inlineStr">
+      <is>
+        <t>Monday</t>
+      </is>
+    </oc>
+    <nc r="E23" t="inlineStr">
+      <is>
+        <t>Tuesday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="238" sId="6">
+    <oc r="A24" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A24" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="239" sId="6">
+    <oc r="A25" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A25" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="240" sId="6">
+    <oc r="A26" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A26" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="241" sId="6" numFmtId="19">
+    <oc r="B26">
+      <v>41310</v>
+    </oc>
+    <nc r="B26">
+      <v>41311</v>
+    </nc>
+  </rcc>
+  <rcc rId="242" sId="6">
+    <oc r="D26">
+      <v>41310</v>
+    </oc>
+    <nc r="D26">
+      <v>41311</v>
+    </nc>
+  </rcc>
+  <rcc rId="243" sId="6">
+    <oc r="E26" t="inlineStr">
+      <is>
+        <t>Tuesday</t>
+      </is>
+    </oc>
+    <nc r="E26" t="inlineStr">
+      <is>
+        <t>Wednesday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="244" sId="6">
+    <oc r="A27" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A27" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="245" sId="6">
+    <oc r="A28" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A28" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="246" sId="6">
+    <oc r="A29" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A29" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="247" sId="6" numFmtId="19">
+    <oc r="B29">
+      <v>41311</v>
+    </oc>
+    <nc r="B29">
+      <v>41312</v>
+    </nc>
+  </rcc>
+  <rcc rId="248" sId="6">
+    <oc r="D29">
+      <v>41311</v>
+    </oc>
+    <nc r="D29">
+      <v>41312</v>
+    </nc>
+  </rcc>
+  <rcc rId="249" sId="6">
+    <oc r="E29" t="inlineStr">
+      <is>
+        <t>Wednesday</t>
+      </is>
+    </oc>
+    <nc r="E29" t="inlineStr">
+      <is>
+        <t>Thursday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="250" sId="6">
+    <oc r="A30" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A30" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="251" sId="6">
+    <oc r="A31" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A31" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="252" sId="6">
+    <oc r="A32" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A32" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="253" sId="6" numFmtId="19">
+    <oc r="B32">
+      <v>41312</v>
+    </oc>
+    <nc r="B32">
+      <v>41313</v>
+    </nc>
+  </rcc>
+  <rcc rId="254" sId="6">
+    <oc r="D32">
+      <v>41312</v>
+    </oc>
+    <nc r="D32">
+      <v>41313</v>
+    </nc>
+  </rcc>
+  <rcc rId="255" sId="6">
+    <oc r="E32" t="inlineStr">
+      <is>
+        <t>Thursday</t>
+      </is>
+    </oc>
+    <nc r="E32" t="inlineStr">
+      <is>
+        <t>Friday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="256" sId="6">
+    <oc r="A33" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A33" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="257" sId="6">
+    <oc r="A34" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A34" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="258" sId="6">
+    <oc r="A35" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A35" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="259" sId="6" numFmtId="19">
+    <oc r="B35">
+      <v>41313</v>
+    </oc>
+    <nc r="B35">
+      <v>41314</v>
+    </nc>
+  </rcc>
+  <rcc rId="260" sId="6">
+    <oc r="D35">
+      <v>41313</v>
+    </oc>
+    <nc r="D35">
+      <v>41314</v>
+    </nc>
+  </rcc>
+  <rcc rId="261" sId="6">
+    <oc r="E35" t="inlineStr">
+      <is>
+        <t>Friday</t>
+      </is>
+    </oc>
+    <nc r="E35" t="inlineStr">
+      <is>
+        <t>Saturday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="262" sId="6">
+    <oc r="A36" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A36" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="263" sId="6">
+    <oc r="A37" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A37" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="264" sId="6">
+    <oc r="A38" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A38" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="265" sId="6" numFmtId="19">
+    <oc r="B38">
+      <v>41314</v>
+    </oc>
+    <nc r="B38">
+      <v>41315</v>
+    </nc>
+  </rcc>
+  <rcc rId="266" sId="6">
+    <oc r="D38">
+      <v>41314</v>
+    </oc>
+    <nc r="D38">
+      <v>41315</v>
+    </nc>
+  </rcc>
+  <rcc rId="267" sId="6">
+    <oc r="E38" t="inlineStr">
+      <is>
+        <t>Saturday</t>
+      </is>
+    </oc>
+    <nc r="E38" t="inlineStr">
+      <is>
+        <t>Sunday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="268" sId="6">
+    <oc r="A39" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A39" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="269" sId="6">
+    <oc r="A40" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A40" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="270" sId="6">
+    <oc r="A41" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A41" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="271" sId="6" numFmtId="19">
+    <oc r="B41">
+      <v>41315</v>
+    </oc>
+    <nc r="B41">
+      <v>41316</v>
+    </nc>
+  </rcc>
+  <rcc rId="272" sId="6">
+    <oc r="D41">
+      <v>41315</v>
+    </oc>
+    <nc r="D41">
+      <v>41316</v>
+    </nc>
+  </rcc>
+  <rcc rId="273" sId="6">
+    <oc r="E41" t="inlineStr">
+      <is>
+        <t>Sunday</t>
+      </is>
+    </oc>
+    <nc r="E41" t="inlineStr">
+      <is>
+        <t>Monday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="274" sId="6">
+    <oc r="A42" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A42" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="275" sId="6">
+    <oc r="A43" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A43" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="276" sId="6">
+    <oc r="A44" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A44" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="277" sId="6" numFmtId="19">
+    <oc r="B44">
+      <v>41316</v>
+    </oc>
+    <nc r="B44">
+      <v>41317</v>
+    </nc>
+  </rcc>
+  <rcc rId="278" sId="6">
+    <oc r="D44">
+      <v>41316</v>
+    </oc>
+    <nc r="D44">
+      <v>41317</v>
+    </nc>
+  </rcc>
+  <rcc rId="279" sId="6">
+    <oc r="E44" t="inlineStr">
+      <is>
+        <t>Monday</t>
+      </is>
+    </oc>
+    <nc r="E44" t="inlineStr">
+      <is>
+        <t>Tuesday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="280" sId="6">
+    <oc r="A45" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A45" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="281" sId="6">
+    <oc r="A46" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A46" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="282" sId="6">
+    <oc r="A47" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A47" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="283" sId="6" numFmtId="19">
+    <oc r="B47">
+      <v>41317</v>
+    </oc>
+    <nc r="B47">
+      <v>41318</v>
+    </nc>
+  </rcc>
+  <rcc rId="284" sId="6">
+    <oc r="D47">
+      <v>41317</v>
+    </oc>
+    <nc r="D47">
+      <v>41318</v>
+    </nc>
+  </rcc>
+  <rcc rId="285" sId="6">
+    <oc r="E47" t="inlineStr">
+      <is>
+        <t>Tuesday</t>
+      </is>
+    </oc>
+    <nc r="E47" t="inlineStr">
+      <is>
+        <t>Wednesday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="286" sId="6">
+    <oc r="A48" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A48" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="287" sId="6">
+    <oc r="A49" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A49" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="288" sId="6">
+    <oc r="A50" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A50" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="289" sId="6" numFmtId="19">
+    <oc r="B50">
+      <v>41318</v>
+    </oc>
+    <nc r="B50">
+      <v>41319</v>
+    </nc>
+  </rcc>
+  <rcc rId="290" sId="6">
+    <oc r="D50">
+      <v>41318</v>
+    </oc>
+    <nc r="D50">
+      <v>41319</v>
+    </nc>
+  </rcc>
+  <rcc rId="291" sId="6">
+    <oc r="E50" t="inlineStr">
+      <is>
+        <t>Wednesday</t>
+      </is>
+    </oc>
+    <nc r="E50" t="inlineStr">
+      <is>
+        <t>Thursday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="292" sId="6">
+    <oc r="A51" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A51" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="293" sId="6">
+    <oc r="A52" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A52" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="294" sId="6">
+    <oc r="A53" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A53" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="295" sId="6" numFmtId="19">
+    <oc r="B53">
+      <v>41319</v>
+    </oc>
+    <nc r="B53">
+      <v>41320</v>
+    </nc>
+  </rcc>
+  <rcc rId="296" sId="6">
+    <oc r="D53">
+      <v>41319</v>
+    </oc>
+    <nc r="D53">
+      <v>41320</v>
+    </nc>
+  </rcc>
+  <rcc rId="297" sId="6">
+    <oc r="E53" t="inlineStr">
+      <is>
+        <t>Thursday</t>
+      </is>
+    </oc>
+    <nc r="E53" t="inlineStr">
+      <is>
+        <t>Friday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="298" sId="6">
+    <oc r="A54" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A54" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="299" sId="6">
+    <oc r="A55" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A55" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="300" sId="6">
+    <oc r="A56" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A56" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="301" sId="6" numFmtId="19">
+    <oc r="B56">
+      <v>41320</v>
+    </oc>
+    <nc r="B56">
+      <v>41321</v>
+    </nc>
+  </rcc>
+  <rcc rId="302" sId="6">
+    <oc r="D56">
+      <v>41320</v>
+    </oc>
+    <nc r="D56">
+      <v>41321</v>
+    </nc>
+  </rcc>
+  <rcc rId="303" sId="6">
+    <oc r="E56" t="inlineStr">
+      <is>
+        <t>Friday</t>
+      </is>
+    </oc>
+    <nc r="E56" t="inlineStr">
+      <is>
+        <t>Saturday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="304" sId="6">
+    <oc r="A57" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A57" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="305" sId="6">
+    <oc r="A58" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A58" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="306" sId="6">
+    <oc r="A59" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A59" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="307" sId="6" numFmtId="19">
+    <oc r="B59">
+      <v>41321</v>
+    </oc>
+    <nc r="B59">
+      <v>41322</v>
+    </nc>
+  </rcc>
+  <rcc rId="308" sId="6">
+    <oc r="D59">
+      <v>41321</v>
+    </oc>
+    <nc r="D59">
+      <v>41322</v>
+    </nc>
+  </rcc>
+  <rcc rId="309" sId="6">
+    <oc r="E59" t="inlineStr">
+      <is>
+        <t>Saturday</t>
+      </is>
+    </oc>
+    <nc r="E59" t="inlineStr">
+      <is>
+        <t>Sunday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="310" sId="6">
+    <oc r="A60" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A60" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="311" sId="6">
+    <oc r="A61" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A61" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="312" sId="6">
+    <oc r="A62" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A62" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="313" sId="6" numFmtId="19">
+    <oc r="B62">
+      <v>41322</v>
+    </oc>
+    <nc r="B62">
+      <v>41323</v>
+    </nc>
+  </rcc>
+  <rcc rId="314" sId="6">
+    <oc r="D62">
+      <v>41322</v>
+    </oc>
+    <nc r="D62">
+      <v>41323</v>
+    </nc>
+  </rcc>
+  <rcc rId="315" sId="6">
+    <oc r="E62" t="inlineStr">
+      <is>
+        <t>Sunday</t>
+      </is>
+    </oc>
+    <nc r="E62" t="inlineStr">
+      <is>
+        <t>Monday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="316" sId="6">
+    <oc r="A63" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A63" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="317" sId="6">
+    <oc r="A64" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A64" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="318" sId="6">
+    <oc r="A65" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A65" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="319" sId="6" numFmtId="19">
+    <oc r="B65">
+      <v>41323</v>
+    </oc>
+    <nc r="B65">
+      <v>41324</v>
+    </nc>
+  </rcc>
+  <rcc rId="320" sId="6">
+    <oc r="D65">
+      <v>41323</v>
+    </oc>
+    <nc r="D65">
+      <v>41324</v>
+    </nc>
+  </rcc>
+  <rcc rId="321" sId="6">
+    <oc r="E65" t="inlineStr">
+      <is>
+        <t>Monday</t>
+      </is>
+    </oc>
+    <nc r="E65" t="inlineStr">
+      <is>
+        <t>Tuesday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="322" sId="6">
+    <oc r="A66" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A66" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="323" sId="6">
+    <oc r="A67" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A67" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="324" sId="6">
+    <oc r="A68" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A68" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="325" sId="6" numFmtId="19">
+    <oc r="B68">
+      <v>41324</v>
+    </oc>
+    <nc r="B68">
+      <v>41325</v>
+    </nc>
+  </rcc>
+  <rcc rId="326" sId="6">
+    <oc r="D68">
+      <v>41324</v>
+    </oc>
+    <nc r="D68">
+      <v>41325</v>
+    </nc>
+  </rcc>
+  <rcc rId="327" sId="6">
+    <oc r="E68" t="inlineStr">
+      <is>
+        <t>Tuesday</t>
+      </is>
+    </oc>
+    <nc r="E68" t="inlineStr">
+      <is>
+        <t>Wednesday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="328" sId="6">
+    <oc r="A69" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A69" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="329" sId="6">
+    <oc r="A70" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A70" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="330" sId="6">
+    <oc r="A71" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A71" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="331" sId="6" numFmtId="19">
+    <oc r="B71">
+      <v>41325</v>
+    </oc>
+    <nc r="B71">
+      <v>41326</v>
+    </nc>
+  </rcc>
+  <rcc rId="332" sId="6">
+    <oc r="D71">
+      <v>41325</v>
+    </oc>
+    <nc r="D71">
+      <v>41326</v>
+    </nc>
+  </rcc>
+  <rcc rId="333" sId="6">
+    <oc r="E71" t="inlineStr">
+      <is>
+        <t>Wednesday</t>
+      </is>
+    </oc>
+    <nc r="E71" t="inlineStr">
+      <is>
+        <t>Thursday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="334" sId="6">
+    <oc r="A72" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A72" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="335" sId="6">
+    <oc r="A73" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A73" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="336" sId="6">
+    <oc r="A74" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A74" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="337" sId="6" numFmtId="19">
+    <oc r="B74">
+      <v>41326</v>
+    </oc>
+    <nc r="B74">
+      <v>41327</v>
+    </nc>
+  </rcc>
+  <rcc rId="338" sId="6">
+    <oc r="D74">
+      <v>41326</v>
+    </oc>
+    <nc r="D74">
+      <v>41327</v>
+    </nc>
+  </rcc>
+  <rcc rId="339" sId="6">
+    <oc r="E74" t="inlineStr">
+      <is>
+        <t>Thursday</t>
+      </is>
+    </oc>
+    <nc r="E74" t="inlineStr">
+      <is>
+        <t>Friday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="340" sId="6">
+    <oc r="A75" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A75" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="341" sId="6">
+    <oc r="A76" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A76" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="342" sId="6">
+    <oc r="A77" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A77" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="343" sId="6" numFmtId="19">
+    <oc r="B77">
+      <v>41327</v>
+    </oc>
+    <nc r="B77">
+      <v>41328</v>
+    </nc>
+  </rcc>
+  <rcc rId="344" sId="6">
+    <oc r="D77">
+      <v>41327</v>
+    </oc>
+    <nc r="D77">
+      <v>41328</v>
+    </nc>
+  </rcc>
+  <rcc rId="345" sId="6">
+    <oc r="E77" t="inlineStr">
+      <is>
+        <t>Friday</t>
+      </is>
+    </oc>
+    <nc r="E77" t="inlineStr">
+      <is>
+        <t>Saturday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="346" sId="6">
+    <oc r="A78" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A78" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="347" sId="6">
+    <oc r="A79" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A79" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="348" sId="6">
+    <oc r="A80" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A80" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="349" sId="6" numFmtId="19">
+    <oc r="B80">
+      <v>41328</v>
+    </oc>
+    <nc r="B80">
+      <v>41329</v>
+    </nc>
+  </rcc>
+  <rcc rId="350" sId="6">
+    <oc r="D80">
+      <v>41328</v>
+    </oc>
+    <nc r="D80">
+      <v>41329</v>
+    </nc>
+  </rcc>
+  <rcc rId="351" sId="6">
+    <oc r="E80" t="inlineStr">
+      <is>
+        <t>Saturday</t>
+      </is>
+    </oc>
+    <nc r="E80" t="inlineStr">
+      <is>
+        <t>Sunday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="352" sId="6">
+    <oc r="A81" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A81" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="353" sId="6">
+    <oc r="A82" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A82" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="354" sId="6">
+    <oc r="A83" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A83" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="355" sId="6" numFmtId="19">
+    <oc r="B83">
+      <v>41329</v>
+    </oc>
+    <nc r="B83">
+      <v>41330</v>
+    </nc>
+  </rcc>
+  <rcc rId="356" sId="6">
+    <oc r="D83">
+      <v>41329</v>
+    </oc>
+    <nc r="D83">
+      <v>41330</v>
+    </nc>
+  </rcc>
+  <rcc rId="357" sId="6">
+    <oc r="E83" t="inlineStr">
+      <is>
+        <t>Sunday</t>
+      </is>
+    </oc>
+    <nc r="E83" t="inlineStr">
+      <is>
+        <t>Monday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="358" sId="6">
+    <oc r="A84" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A84" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="359" sId="6">
+    <oc r="A85" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A85" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="360" sId="6">
+    <oc r="A86" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A86" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="361" sId="6" numFmtId="19">
+    <oc r="B86">
+      <v>41330</v>
+    </oc>
+    <nc r="B86">
+      <v>41331</v>
+    </nc>
+  </rcc>
+  <rcc rId="362" sId="6">
+    <oc r="D86">
+      <v>41330</v>
+    </oc>
+    <nc r="D86">
+      <v>41331</v>
+    </nc>
+  </rcc>
+  <rcc rId="363" sId="6">
+    <oc r="E86" t="inlineStr">
+      <is>
+        <t>Monday</t>
+      </is>
+    </oc>
+    <nc r="E86" t="inlineStr">
+      <is>
+        <t>Tuesday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="364" sId="6">
+    <oc r="A87" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A87" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="365" sId="6">
+    <oc r="A88" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A88" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="366" sId="6">
+    <oc r="A89" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A89" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="367" sId="6" numFmtId="19">
+    <oc r="B89">
+      <v>41331</v>
+    </oc>
+    <nc r="B89">
+      <v>41332</v>
+    </nc>
+  </rcc>
+  <rcc rId="368" sId="6">
+    <oc r="D89">
+      <v>41331</v>
+    </oc>
+    <nc r="D89">
+      <v>41332</v>
+    </nc>
+  </rcc>
+  <rcc rId="369" sId="6">
+    <oc r="E89" t="inlineStr">
+      <is>
+        <t>Tuesday</t>
+      </is>
+    </oc>
+    <nc r="E89" t="inlineStr">
+      <is>
+        <t>Wednesday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="370" sId="6">
+    <oc r="A90" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A90" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="371" sId="6">
+    <oc r="A91" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A91" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="372" sId="6">
+    <oc r="A92" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A92" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="373" sId="6" numFmtId="19">
+    <oc r="B92">
+      <v>41332</v>
+    </oc>
+    <nc r="B92">
+      <v>41333</v>
+    </nc>
+  </rcc>
+  <rcc rId="374" sId="6">
+    <oc r="D92">
+      <v>41332</v>
+    </oc>
+    <nc r="D92">
+      <v>41333</v>
+    </nc>
+  </rcc>
+  <rcc rId="375" sId="6">
+    <oc r="E92" t="inlineStr">
+      <is>
+        <t>Wednesday</t>
+      </is>
+    </oc>
+    <nc r="E92" t="inlineStr">
+      <is>
+        <t>Thursday</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="376" sId="6">
+    <oc r="A93" t="inlineStr">
+      <is>
+        <t>breakfast</t>
+      </is>
+    </oc>
+    <nc r="A93" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="377" sId="6">
+    <oc r="A94" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A94" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="378" sId="6">
+    <oc r="C94">
+      <v>564</v>
+    </oc>
+    <nc r="C94">
+      <v>16</v>
+    </nc>
+  </rcc>
+  <rcc rId="379" sId="6">
+    <oc r="A95" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </oc>
+    <nc r="A95" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="380" sId="6">
+    <oc r="A97" t="inlineStr">
+      <is>
+        <t>lunch</t>
+      </is>
+    </oc>
+    <nc r="A97" t="inlineStr">
+      <is>
+        <t>dinner</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="6" sqref="D97" start="0" length="0">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+  </rfmt>
+  <rfmt sheetId="6" sqref="D97">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="2">
+  <userInfo guid="{CDC0E8B4-BCE5-4D3F-8424-F8C784956298}" name="Network Student" id="-248520132" dateTime="2013-02-28T23:23:33"/>
+  <userInfo guid="{75126F2E-4F5C-48EE-88DD-C6E32F8F7E3A}" name="Network Student" id="-248570193" dateTime="2013-02-28T23:27:41"/>
+</users>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -799,7 +5178,7 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{292070CA-CCC0-4443-AE30-5245732CEFEF}">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E2" sqref="E2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -915,10 +5294,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -926,29 +5305,63 @@
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="2">
         <v>38751.524259259262</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4">
+        <v>38751</v>
+      </c>
+      <c r="E2" s="5">
+        <f>MATCH("*",A2:A3,-1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2">
+        <v>41333</v>
+      </c>
+      <c r="C3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="4">
+        <v>41333</v>
+      </c>
     </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{292070CA-CCC0-4443-AE30-5245732CEFEF}">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B13" sqref="B13"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -958,10 +5371,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E97"/>
+  <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="C97" sqref="C97"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2622,7 +7035,16 @@
         <v>39</v>
       </c>
     </row>
+    <row r="98" spans="1:5">
+      <c r="B98" s="2"/>
+    </row>
   </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{292070CA-CCC0-4443-AE30-5245732CEFEF}">
+      <selection activeCell="F5" sqref="F5"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+  </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>